<commit_message>
South Dakota water rights update.
South Dakota water rights update.
</commit_message>
<xml_diff>
--- a/SouthDakota/WaterAllocation/SD_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/SouthDakota/WaterAllocation/SD_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\SouthDakota\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64C0FD7-2454-4B66-90A7-3F464FF2800E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ED6AE5-E791-4D4A-ADFB-D2CD5B47C4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="714" activeTab="3" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="5" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="301">
   <si>
     <t>Name</t>
   </si>
@@ -872,9 +872,6 @@
     <t>COUNTY_1</t>
   </si>
   <si>
-    <t>BASIN</t>
-  </si>
-  <si>
     <t>It would be nice to have the list of translated abbrevations for watersources &amp; site information.</t>
   </si>
   <si>
@@ -930,6 +927,21 @@
   </si>
   <si>
     <t>HYDROUNIT1</t>
+  </si>
+  <si>
+    <t>tweaked lats name entry to not contain "CITY OF", but first name entry does.</t>
+  </si>
+  <si>
+    <t>Removed commas form last and first name, repace with &amp;.</t>
+  </si>
+  <si>
+    <t>OwnerClassificationCV</t>
+  </si>
+  <si>
+    <t>Army (USA)</t>
+  </si>
+  <si>
+    <t>WSWC defined owner tag.</t>
   </si>
 </sst>
 </file>
@@ -1705,7 +1717,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2009,6 +2021,18 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2368,8 +2392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2410,17 +2434,27 @@
         <v>251</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="97" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="97" t="s">
+        <v>297</v>
+      </c>
+    </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="43" t="s">
         <v>242</v>
       </c>
       <c r="B17" s="93" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" s="97" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2537,7 +2571,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="92" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F4" s="61" t="s">
         <v>38</v>
@@ -2569,7 +2603,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F5" s="46" t="s">
         <v>38</v>
@@ -2601,7 +2635,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F6" s="46" t="s">
         <v>38</v>
@@ -2633,7 +2667,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F7" s="46" t="s">
         <v>38</v>
@@ -2665,7 +2699,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F8" s="46" t="s">
         <v>38</v>
@@ -2697,7 +2731,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F9" s="46" t="s">
         <v>38</v>
@@ -2727,7 +2761,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F10" s="46" t="s">
         <v>38</v>
@@ -2759,7 +2793,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="100" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F11" s="46" t="s">
         <v>38</v>
@@ -2791,7 +2825,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F12" s="46" t="s">
         <v>38</v>
@@ -2926,7 +2960,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="94" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>38</v>
@@ -2986,7 +3020,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="95" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F6" s="46" t="s">
         <v>38</v>
@@ -3178,7 +3212,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="95" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F12" s="46" t="s">
         <v>38</v>
@@ -3210,7 +3244,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="95" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F13" s="46" t="s">
         <v>38</v>
@@ -3241,7 +3275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8BA2FE-2555-4166-A4DF-0203EE1C77D7}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -3662,7 +3696,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3757,7 +3791,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F4" s="61" t="s">
         <v>38</v>
@@ -3787,7 +3821,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F5" s="44" t="s">
         <v>38</v>
@@ -3817,7 +3851,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F6" s="44" t="s">
         <v>38</v>
@@ -3876,12 +3910,14 @@
       <c r="D8" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="24"/>
+      <c r="E8" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="F8" s="42" t="s">
         <v>264</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="H8" s="82"/>
       <c r="I8" s="75" t="s">
@@ -3905,7 +3941,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>38</v>
@@ -3921,7 +3957,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>43</v>
       </c>
@@ -3935,13 +3971,13 @@
         <v>20</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>38</v>
+        <v>269</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>264</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>38</v>
+        <v>268</v>
       </c>
       <c r="H10" s="82"/>
       <c r="I10" s="75" t="s">
@@ -3972,8 +4008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E7F0DF-14BE-4BB8-BB6C-8815808B0B66}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4072,7 +4108,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="66" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F4" s="61" t="s">
         <v>38</v>
@@ -4102,7 +4138,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F5" s="46" t="s">
         <v>38</v>
@@ -4132,7 +4168,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F6" s="46" t="s">
         <v>38</v>
@@ -4222,7 +4258,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F9" s="46" t="s">
         <v>38</v>
@@ -4250,7 +4286,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F10" s="46" t="s">
         <v>38</v>
@@ -4280,7 +4316,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F11" s="46" t="s">
         <v>38</v>
@@ -4316,7 +4352,7 @@
         <v>264</v>
       </c>
       <c r="G12" s="47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H12" s="80"/>
       <c r="I12" s="81" t="s">
@@ -4400,7 +4436,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F15" s="46" t="s">
         <v>38</v>
@@ -4430,7 +4466,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F16" s="46" t="s">
         <v>38</v>
@@ -4486,13 +4522,13 @@
         <v>38</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="42" t="s">
-        <v>264</v>
-      </c>
-      <c r="G18" s="48" t="s">
-        <v>270</v>
+        <v>282</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="47" t="s">
+        <v>38</v>
       </c>
       <c r="H18" s="80"/>
       <c r="I18" s="79" t="s">
@@ -4516,7 +4552,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F19" s="46" t="s">
         <v>38</v>
@@ -4546,7 +4582,7 @@
         <v>38</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F20" s="46" t="s">
         <v>38</v>
@@ -4576,13 +4612,13 @@
         <v>20</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>264</v>
+        <v>282</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>268</v>
+        <v>38</v>
       </c>
       <c r="H21" s="80"/>
       <c r="I21" s="79" t="s">
@@ -4636,7 +4672,7 @@
         <v>38</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F23" s="46" t="s">
         <v>38</v>
@@ -4663,10 +4699,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4923,7 +4959,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="102" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>38</v>
@@ -4987,7 +5023,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>38</v>
@@ -5019,7 +5055,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="68" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>38</v>
@@ -5051,7 +5087,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="69" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F13" s="61" t="s">
         <v>38</v>
@@ -5083,7 +5119,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>38</v>
@@ -5115,7 +5151,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>38</v>
@@ -5147,7 +5183,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>38</v>
@@ -5179,7 +5215,7 @@
         <v>20</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>38</v>
@@ -5211,7 +5247,7 @@
         <v>38</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>38</v>
@@ -5243,7 +5279,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>38</v>
@@ -5275,7 +5311,7 @@
         <v>38</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>38</v>
@@ -5307,7 +5343,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>38</v>
@@ -5409,7 +5445,7 @@
         <v>264</v>
       </c>
       <c r="G24" s="48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H24" s="87" t="s">
         <v>38</v>
@@ -5435,7 +5471,7 @@
         <v>38</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F25" s="42" t="s">
         <v>264</v>
@@ -5499,7 +5535,7 @@
         <v>20</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>38</v>
@@ -5531,7 +5567,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F28" s="24" t="s">
         <v>38</v>
@@ -5563,7 +5599,7 @@
         <v>38</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F29" s="24" t="s">
         <v>38</v>
@@ -5595,7 +5631,7 @@
         <v>20</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F30" s="46" t="s">
         <v>38</v>
@@ -5627,7 +5663,7 @@
         <v>38</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>38</v>
@@ -5677,7 +5713,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="35" t="s">
         <v>101</v>
       </c>
@@ -5691,7 +5727,7 @@
         <v>38</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F33" s="24" t="s">
         <v>38</v>
@@ -5709,7 +5745,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="35" t="s">
         <v>98</v>
       </c>
@@ -5723,7 +5759,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F34" s="24" t="s">
         <v>38</v>
@@ -5741,7 +5777,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>100</v>
       </c>
@@ -5755,7 +5791,7 @@
         <v>20</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F35" s="24" t="s">
         <v>38</v>
@@ -5773,7 +5809,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>154</v>
       </c>
@@ -5805,7 +5841,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="35" t="s">
         <v>82</v>
       </c>
@@ -5819,7 +5855,7 @@
         <v>38</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F37" s="24" t="s">
         <v>38</v>
@@ -5837,7 +5873,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="72" t="s">
         <v>245</v>
       </c>
@@ -5863,7 +5899,7 @@
       <c r="I38" s="90"/>
       <c r="J38" s="83"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="35" t="s">
         <v>90</v>
       </c>
@@ -5877,7 +5913,7 @@
         <v>38</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F39" s="24" t="s">
         <v>38</v>
@@ -5895,7 +5931,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
         <v>91</v>
       </c>
@@ -5925,7 +5961,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="35" t="s">
         <v>99</v>
       </c>
@@ -5939,7 +5975,7 @@
         <v>20</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F41" s="24" t="s">
         <v>38</v>
@@ -5957,7 +5993,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="35" t="s">
         <v>96</v>
       </c>
@@ -5971,7 +6007,7 @@
         <v>38</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F42" s="24" t="s">
         <v>38</v>
@@ -5989,53 +6025,53 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="35" t="s">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="104"/>
+      <c r="H43" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="I43" s="106" t="s">
+        <v>299</v>
+      </c>
+      <c r="J43" s="107" t="s">
+        <v>300</v>
+      </c>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B44" s="36" t="s">
         <v>33</v>
-      </c>
-      <c r="C43" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>279</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="H43" s="87" t="s">
-        <v>38</v>
-      </c>
-      <c r="I43" s="88" t="s">
-        <v>38</v>
-      </c>
-      <c r="J43" s="76" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" s="36" t="s">
-        <v>16</v>
       </c>
       <c r="C44" s="36" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F44" s="24" t="s">
         <v>38</v>
@@ -6046,80 +6082,112 @@
       <c r="H44" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="79" t="s">
-        <v>133</v>
-      </c>
-      <c r="J44" s="83" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I44" s="88" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="76" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="35" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="36" t="s">
         <v>18</v>
       </c>
       <c r="D45" s="39" t="s">
         <v>20</v>
       </c>
       <c r="E45" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="79" t="s">
+        <v>133</v>
+      </c>
+      <c r="J45" s="83" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="F45" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G45" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="H45" s="87" t="s">
-        <v>38</v>
-      </c>
-      <c r="I45" s="79" t="s">
+      <c r="F46" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G46" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="I46" s="79" t="s">
         <v>132</v>
       </c>
-      <c r="J45" s="76" t="s">
+      <c r="J46" s="76" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="35" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B47" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="C47" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>279</v>
-      </c>
-      <c r="F46" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G46" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="H46" s="87" t="s">
-        <v>38</v>
-      </c>
-      <c r="I46" s="79" t="s">
+      <c r="D47" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="I47" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="J46" s="76" t="s">
+      <c r="J47" s="76" t="s">
         <v>210</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:P46">
-    <sortCondition ref="A14:A46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:P47">
+    <sortCondition ref="A14:A47"/>
   </sortState>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>